<commit_message>
add user avatar api
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -21,7 +21,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="E11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0">
+    <comment ref="E12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="127">
   <si>
     <t>check if register</t>
   </si>
@@ -1023,6 +1023,49 @@
  /* the message id */
  "friend_mobile": xxx,
  "mesg_id": xxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>download avatar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/download_avatar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upload avatar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user/upload_avatar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "mobile": xxxx,
+ "avatar": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "mobile": xxxx,
+ "avatar_id": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "avatar": xxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "status": 0,
+ "avatar_id": xxx,
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1296,7 +1339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1408,6 +1451,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1509,8 +1571,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B2:G13" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
-  <autoFilter ref="B2:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B2:G15" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="B2:G15"/>
   <tableColumns count="6">
     <tableColumn id="1" name="模块" dataDxfId="6"/>
     <tableColumn id="2" name="说明" dataDxfId="5"/>
@@ -1821,10 +1883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I13"/>
+  <dimension ref="B2:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1921,157 +1983,191 @@
       </c>
       <c r="H5" s="36"/>
     </row>
-    <row r="6" spans="2:9" ht="99.95" customHeight="1">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="2:9" s="51" customFormat="1" ht="99.95" customHeight="1">
+      <c r="B6" s="45"/>
+      <c r="C6" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="49"/>
+      <c r="H6" s="50"/>
+    </row>
+    <row r="7" spans="2:9" s="51" customFormat="1" ht="99.95" customHeight="1" thickBot="1">
+      <c r="B7" s="45"/>
+      <c r="C7" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="49"/>
+      <c r="H7" s="50"/>
+    </row>
+    <row r="8" spans="2:9" ht="99.95" customHeight="1">
+      <c r="B8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H8" s="34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="99.95" customHeight="1">
-      <c r="B7" s="2"/>
-      <c r="C7" s="10" t="s">
+    <row r="9" spans="2:9" ht="99.95" customHeight="1">
+      <c r="B9" s="2"/>
+      <c r="C9" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H9" s="35" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="173.25" customHeight="1">
-      <c r="B8" s="23"/>
-      <c r="C8" s="24" t="s">
+    <row r="10" spans="2:9" ht="173.25" customHeight="1">
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D10" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E10" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F10" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="2:9" ht="96" customHeight="1">
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
+      <c r="G10" s="37"/>
+      <c r="H10" s="35"/>
+    </row>
+    <row r="11" spans="2:9" ht="96" customHeight="1">
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D11" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E11" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F11" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="35"/>
-    </row>
-    <row r="10" spans="2:9" s="42" customFormat="1" ht="96" customHeight="1">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39" t="s">
+      <c r="G11" s="25"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="2:9" s="42" customFormat="1" ht="96" customHeight="1">
+      <c r="B12" s="38"/>
+      <c r="C12" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D12" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E12" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F12" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="2:9" ht="83.25" customHeight="1" thickBot="1">
-      <c r="B11" s="2"/>
-      <c r="C11" s="10" t="s">
+      <c r="G12" s="40"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="2:9" ht="83.25" customHeight="1" thickBot="1">
+      <c r="B13" s="2"/>
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="176.25" thickBot="1">
-      <c r="B12" s="2" t="s">
+    <row r="14" spans="2:9" ht="176.25" thickBot="1">
+      <c r="B14" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C14" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D14" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E14" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H14" s="34" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="148.5">
-      <c r="B13" s="2"/>
-      <c r="C13" s="12" t="s">
+    <row r="15" spans="2:9" ht="148.5">
+      <c r="B15" s="2"/>
+      <c r="C15" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D15" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E15" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F15" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add notify friend to update position
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
   <si>
     <t>check if register</t>
   </si>
@@ -1189,6 +1189,12 @@
  },
  ]
 }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push Message Format：
+msg content： 303
+extras： 发送方用户名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1597,11 +1603,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2018,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F25" sqref="F18:F25"/>
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2322,7 +2328,7 @@
       </c>
       <c r="G16" s="22"/>
     </row>
-    <row r="17" spans="2:7" ht="229.5">
+    <row r="17" spans="2:8" ht="229.5">
       <c r="B17" s="2"/>
       <c r="C17" s="12" t="s">
         <v>137</v>
@@ -2330,7 +2336,7 @@
       <c r="D17" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="51" t="s">
         <v>139</v>
       </c>
       <c r="F17" s="43" t="s">
@@ -2338,7 +2344,7 @@
       </c>
       <c r="G17" s="22"/>
     </row>
-    <row r="18" spans="2:7" ht="108">
+    <row r="18" spans="2:8" ht="108">
       <c r="B18" s="2"/>
       <c r="C18" s="12" t="s">
         <v>128</v>
@@ -2353,6 +2359,9 @@
         <v>136</v>
       </c>
       <c r="G18" s="22"/>
+      <c r="H18" s="35" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2497,12 +2506,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="109.5" customHeight="1">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="3" spans="2:18">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
add 401 for push return code
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="API 使用说明" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="144">
   <si>
     <t>check if register</t>
   </si>
@@ -1081,14 +1081,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>location_get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>feed/locate_get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{
  /* the mobile that register */
  "mobile": xxxx,
@@ -1195,6 +1187,48 @@
     <t>Push Message Format：
 msg content： 303
 extras： 发送方用户名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feed/locate_update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>location_update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* position already expired, need update by friend */
+ "status": 401</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据过期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1725,8 +1759,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="C2:D12" totalsRowShown="0">
-  <autoFilter ref="C2:D12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="C2:D13" totalsRowShown="0">
+  <autoFilter ref="C2:D13"/>
   <tableColumns count="2">
     <tableColumn id="1" name="返回码" dataDxfId="0"/>
     <tableColumn id="2" name="说明"/>
@@ -2024,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2280,10 +2314,10 @@
         <v>106</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>112</v>
@@ -2301,7 +2335,7 @@
         <v>107</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F15" s="43" t="s">
         <v>114</v>
@@ -2321,46 +2355,48 @@
         <v>127</v>
       </c>
       <c r="E16" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" s="43" t="s">
         <v>131</v>
-      </c>
-      <c r="F16" s="43" t="s">
-        <v>133</v>
       </c>
       <c r="G16" s="22"/>
     </row>
     <row r="17" spans="2:8" ht="229.5">
       <c r="B17" s="2"/>
       <c r="C17" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="F17" s="43" t="s">
         <v>138</v>
-      </c>
-      <c r="E17" s="51" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>140</v>
       </c>
       <c r="G17" s="22"/>
     </row>
     <row r="18" spans="2:8" ht="108">
       <c r="B18" s="2"/>
       <c r="C18" s="12" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="G18" s="22"/>
+        <v>134</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>142</v>
+      </c>
       <c r="H18" s="35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2376,10 +2412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:D12"/>
+  <dimension ref="C2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2414,65 +2450,73 @@
     </row>
     <row r="5" spans="3:4" ht="20.100000000000001" customHeight="1">
       <c r="C5" s="17">
-        <v>14</v>
+        <v>401</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="20.100000000000001" customHeight="1">
       <c r="C6" s="17">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="20.100000000000001" customHeight="1">
       <c r="C7" s="17">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="20.100000000000001" customHeight="1">
       <c r="C8" s="17">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="20.100000000000001" customHeight="1">
       <c r="C9" s="17">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="20.100000000000001" customHeight="1">
       <c r="C10" s="17">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="20.100000000000001" customHeight="1">
       <c r="C11" s="17">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="20.100000000000001" customHeight="1">
+      <c r="C12" s="17">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="3:4">
-      <c r="C12" s="17">
+    <row r="13" spans="3:4">
+      <c r="C13" s="17">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ball and Add profile
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="167">
   <si>
     <t>check if register</t>
   </si>
@@ -1288,28 +1288,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ball/reference_get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>query ball base on location</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>query ball base on reference</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ball Module</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- /* the mobile that register */
- "mobile": xxxx,
- /* the ball id */
- "ball_id": xxx,
-}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1355,20 +1338,106 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Profile Module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>{
  "status": 0,
- "mobile": xxx,
- "ball_lat": xxxx,
- "ball_lng": xxxx,
-}</t>
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>query ball base by users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ball/get_all</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{
- "status": 0,
- "mobile": xxx,
- "ball_lat": xxxx,
- "ball_lng": xxxx,
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the location */
+ "lat": xxx,
+ "lng": xxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profile/get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profile/update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the user blood */
+ "blood_level": xxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the user blood */
+ "blood_level": xxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile":xxx,
+ "balls:":[{
+  /* the mobile that register */
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ },{
+  /* the mobile that register */
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ }]
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1900,8 +1969,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B2:G22" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
-  <autoFilter ref="B2:G22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B2:G23" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="B2:G23"/>
   <tableColumns count="6">
     <tableColumn id="1" name="模块" dataDxfId="6"/>
     <tableColumn id="2" name="说明" dataDxfId="5"/>
@@ -2212,10 +2281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2552,12 +2621,12 @@
         <v>137</v>
       </c>
       <c r="H18" s="35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="216">
       <c r="B19" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>144</v>
@@ -2566,53 +2635,81 @@
         <v>145</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F19" s="43" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="53" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="81">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="337.5">
       <c r="B20" s="2"/>
       <c r="C20" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>146</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="G20" s="22"/>
     </row>
-    <row r="21" spans="2:8" ht="81">
+    <row r="21" spans="2:8" ht="337.5">
       <c r="B21" s="2"/>
       <c r="C21" s="12" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="F21" s="43" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="2"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
+    <row r="22" spans="2:8" ht="81">
+      <c r="B22" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>155</v>
+      </c>
       <c r="G22" s="22"/>
+    </row>
+    <row r="23" spans="2:8" ht="81">
+      <c r="B23" s="2"/>
+      <c r="C23" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add global code for ball notification
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="API 使用说明" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="170">
   <si>
     <t>check if register</t>
   </si>
@@ -1439,6 +1439,18 @@
   "current_lng": xxxx,
  }]
 }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>you hit by ball</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>your ball has hit someone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>your ball hit nothing</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1984,8 +1996,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="C2:D14" totalsRowShown="0">
-  <autoFilter ref="C2:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="C2:D17" totalsRowShown="0">
+  <autoFilter ref="C2:D17"/>
   <tableColumns count="2">
     <tableColumn id="1" name="返回码" dataDxfId="0"/>
     <tableColumn id="2" name="说明"/>
@@ -2283,7 +2295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2724,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:D14"/>
+  <dimension ref="C2:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2838,6 +2850,30 @@
       </c>
       <c r="D14" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4">
+      <c r="C15" s="17">
+        <v>283</v>
+      </c>
+      <c r="D15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4">
+      <c r="C16" s="17">
+        <v>285</v>
+      </c>
+      <c r="D16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" s="17">
+        <v>287</v>
+      </c>
+      <c r="D17" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ball location_get api and Add ball current__loc api
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="API 使用说明" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="174">
   <si>
     <t>check if register</t>
   </si>
@@ -1357,16 +1357,6 @@
   </si>
   <si>
     <t>ball/get_all</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- /* the mobile that register */
- "mobile": xxxx,
- /* the location */
- "lat": xxx,
- "lng": xxx,
-}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1451,6 +1441,68 @@
   </si>
   <si>
     <t>your ball hit nothing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">get ball location </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ball/current_loc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the location */
+ "lat": xxx,
+ "lng": xxx,
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"distance": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the ball id */
+ "ball_id": xxxx
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  /* the mobile that register */
+  "mobile":xxx,
+  "ball_id": xxxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1981,8 +2033,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B2:G23" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
-  <autoFilter ref="B2:G23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B2:G24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="B2:G24"/>
   <tableColumns count="6">
     <tableColumn id="1" name="模块" dataDxfId="6"/>
     <tableColumn id="2" name="说明" dataDxfId="5"/>
@@ -2293,10 +2345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I23"/>
+  <dimension ref="B2:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2657,71 +2709,88 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="337.5">
+    <row r="20" spans="2:8" ht="108">
       <c r="B20" s="2"/>
       <c r="C20" s="12" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G20" s="22"/>
+      <c r="H20" s="53"/>
     </row>
     <row r="21" spans="2:8" ht="337.5">
       <c r="B21" s="2"/>
       <c r="C21" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="F21" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="G21" s="22"/>
+    </row>
+    <row r="22" spans="2:8" ht="337.5">
+      <c r="B22" s="2"/>
+      <c r="C22" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="E21" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="G21" s="22"/>
-    </row>
-    <row r="22" spans="2:8" ht="81">
-      <c r="B22" s="2" t="s">
+      <c r="E22" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="G22" s="22"/>
+    </row>
+    <row r="23" spans="2:8" ht="81">
+      <c r="B23" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>154</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="E22" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G22" s="22"/>
-    </row>
-    <row r="23" spans="2:8" ht="81">
-      <c r="B23" s="2"/>
-      <c r="C23" s="12" t="s">
-        <v>160</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>161</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F23" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" spans="2:8" ht="81">
+      <c r="B24" s="2"/>
+      <c r="C24" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="G23" s="22"/>
+      <c r="F24" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="G24" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2738,7 +2807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2857,7 +2926,7 @@
         <v>283</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="3:4">
@@ -2865,7 +2934,7 @@
         <v>285</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="3:4">
@@ -2873,7 +2942,7 @@
         <v>287</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge locate_get and get_all apis to locate_get
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="179">
   <si>
     <t>check if register</t>
   </si>
@@ -1115,26 +1115,6 @@
   </si>
   <si>
     <t>feed/locate_get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- "status": 0, 
- "mobile": xxx,
- "geo": [ 
- {
- "friend_mobile": xxx
- /* lat and lng */
- "lat": xxx,
- "lng": xxx,
- }, {
- "friend_mobile": xxx
- /* lat and lng */
- "lat": xxx,
- "lng": xxx,
- },
- ]
-}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1391,15 +1371,6 @@
     <t>{
  /* the mobile that register */
  "mobile": xxxx,
- /* the user blood */
- "blood_level": xxx,
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- /* the mobile that register */
- "mobile": xxxx,
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1452,6 +1423,46 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the ball id */
+ "ball_id": xxxx
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  /* the mobile that register */
+  "mobile":xxx,
+  "ball_id": xxxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "status": 0, 
+ "mobile": xxx,
+ "geo": [ 
+ {
+ "friend_mobile": xxx
+ /* lat and lng */
+ "lat": xxx,
+ "lng": xxx,
+ }, {
+ "friend_mobile": xxx
+ /* lat and lng */
+ "lat": xxx,
+ "lng": xxx,
+ },
+ ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">{
  /* the mobile that register */
@@ -1463,45 +1474,107 @@
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF7F7F7F"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"distance": xxx,</t>
+      <t>"distance": xxx,
+}</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-}</t>
-    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get balls base on location
+and users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ball/locate_get</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{
  /* the mobile that register */
  "mobile": xxxx,
- /* the ball id */
- "ball_id": xxxx
+ /* 1: location, 2: user,3 loaction
+ and user,
+ "mask": xxxx,
+ /* the location */
+ "lat": xxx,
+ "lng": xxx,
+ "distance": xxx,
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{
+ /* the mobile that register */
+ "mobile":xxx,
+ "balls:":[{
   /* the mobile that register */
-  "mobile":xxx,
   "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
   /* the location of ball */
   "current_lat": xxxx,
   "current_lng": xxxx,
+ },{
+  /* the mobile that register */
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ }]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "status": 0,
+ /* the mobile that register */
+ "mobile":xxx,
+ "balls:":[{
+  /* the mobile that register */
+  "user": xxx,
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ },{
+  /* the mobile that register */
+  "user": xxx,
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ }]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "status": 0,
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the user blood */
+ "blood_level": xxx,
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1510,7 +1583,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1651,8 +1724,25 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1689,8 +1779,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1788,11 +1884,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1929,12 +2043,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="解释性文本" xfId="1" builtinId="53"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -2033,8 +2160,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B2:G24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
-  <autoFilter ref="B2:G24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B2:G25" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="B2:G25"/>
   <tableColumns count="6">
     <tableColumn id="1" name="模块" dataDxfId="6"/>
     <tableColumn id="2" name="说明" dataDxfId="5"/>
@@ -2345,10 +2472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I24"/>
+  <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2474,7 +2601,7 @@
         <v>119</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G7" s="48"/>
       <c r="H7" s="49"/>
@@ -2603,7 +2730,7 @@
         <v>106</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>129</v>
@@ -2636,16 +2763,16 @@
     <row r="16" spans="2:9" ht="54">
       <c r="B16" s="2"/>
       <c r="C16" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E16" s="43" t="s">
+      <c r="F16" s="43" t="s">
         <v>141</v>
-      </c>
-      <c r="F16" s="43" t="s">
-        <v>142</v>
       </c>
       <c r="G16" s="52"/>
     </row>
@@ -2676,121 +2803,136 @@
         <v>133</v>
       </c>
       <c r="E18" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="F18" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>137</v>
-      </c>
       <c r="H18" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="216">
       <c r="B19" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>145</v>
-      </c>
       <c r="E19" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" s="43" t="s">
         <v>151</v>
-      </c>
-      <c r="F19" s="43" t="s">
-        <v>152</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="53" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="108">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="222" customHeight="1">
       <c r="B20" s="2"/>
       <c r="C20" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="F20" s="43" t="s">
         <v>170</v>
-      </c>
-      <c r="E20" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>173</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="53"/>
     </row>
-    <row r="21" spans="2:8" ht="337.5">
-      <c r="B21" s="2"/>
-      <c r="C21" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="12" t="s">
+    <row r="21" spans="2:8" ht="121.5" customHeight="1">
+      <c r="B21" s="54"/>
+      <c r="C21" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="E21" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="G21" s="22"/>
-    </row>
-    <row r="22" spans="2:8" ht="337.5">
-      <c r="B22" s="2"/>
-      <c r="C22" s="12" t="s">
+      <c r="D21" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="57"/>
+    </row>
+    <row r="22" spans="2:8" ht="120.75" customHeight="1">
+      <c r="B22" s="54"/>
+      <c r="C22" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="E22" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="E22" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="G22" s="22"/>
-    </row>
-    <row r="23" spans="2:8" ht="81">
-      <c r="B23" s="2" t="s">
+      <c r="F22" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="57"/>
+    </row>
+    <row r="23" spans="2:8" s="12" customFormat="1" ht="120.75" customHeight="1">
+      <c r="C23" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="2:8" ht="81">
+      <c r="B24" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="F23" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G23" s="22"/>
-    </row>
-    <row r="24" spans="2:8" ht="81">
-      <c r="B24" s="2"/>
-      <c r="C24" s="12" t="s">
-        <v>159</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>160</v>
       </c>
       <c r="E24" s="43" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G24" s="22"/>
+    </row>
+    <row r="25" spans="2:8" ht="94.5">
+      <c r="B25" s="2"/>
+      <c r="C25" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="G25" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2878,7 +3020,7 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="20.100000000000001" customHeight="1">
@@ -2926,7 +3068,7 @@
         <v>283</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="3:4">
@@ -2934,7 +3076,7 @@
         <v>285</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="3:4">
@@ -2942,7 +3084,7 @@
         <v>287</v>
       </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2975,12 +3117,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="109.5" customHeight="1">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="3" spans="2:18">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
Add push return value
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -1282,14 +1282,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">/* ball got end, notify all reference people */
-Push Message Format：
-msg content： 285
-extras： 发送方用户名
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{
  /* the mobile that register */
  "mobile": xxxx,
@@ -1511,6 +1503,128 @@
   "current_lng": xxxx,
  }]
 }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+  /* the mobile that register */
+  "mobile":xxx,
+  "ball_id": xxxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  /* 0: running, 3: dead */
+  "ball_status": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profile/update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the user blood */
+ "score": xxx,
+}</t>
+  </si>
+  <si>
+    <t>{
+ "status": 0,
+ /* the mobile that register */
+ "mobile": xxxx,
+ /* the user blood */
+ "score": xxx,
+}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* ball got clashed, notify the people that hit by ball*/
+Push Message Format：
+msg content： 285
+extras： {
+/* the people name that ball hit */
+"receiver": xxx,
+"end_lat": xxxx,
+"end_lng": xxxx,
+"ball_id": xxxx,
+}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/* ball got clashed, notify the people that own the ball*/
+Push Message Format：
+msg content： 283
+extras： {
+/* the people name that ball own */
+"receiver": xxx,
+"end_lat": xxxx,
+"end_lng": xxxx,
+"ball_id": xxxx,
+}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1544,69 +1658,12 @@
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <r>
-      <t xml:space="preserve">{
-  /* the mobile that register */
-  "mobile":xxx,
-  "ball_id": xxxx,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  /* 0: running, 3: dead */
-  "ball_status": xxx,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-  /* the location of ball */
-  "current_lat": xxxx,
-  "current_lng": xxxx,
-}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>profile/update</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- /* the mobile that register */
- "mobile": xxxx,
- /* the user blood */
- "score": xxx,
-}</t>
-  </si>
-  <si>
-    <t>{
- "status": 0,
- /* the mobile that register */
- "mobile": xxxx,
- /* the user blood */
- "score": xxx,
-}</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1761,6 +1818,22 @@
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1929,7 +2002,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2078,22 +2151,25 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2510,8 +2586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2521,8 +2597,9 @@
     <col min="4" max="4" width="27.75" style="12" customWidth="1"/>
     <col min="5" max="5" width="40.5" style="22" customWidth="1"/>
     <col min="6" max="6" width="33.25" style="22" customWidth="1"/>
-    <col min="7" max="7" width="56.375" customWidth="1"/>
+    <col min="7" max="7" width="45" customWidth="1"/>
     <col min="8" max="8" width="56.375" style="17" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="14.25" thickBot="1">
@@ -2812,7 +2889,7 @@
       </c>
       <c r="G16" s="52"/>
     </row>
-    <row r="17" spans="2:8" ht="94.5">
+    <row r="17" spans="2:9" ht="94.5">
       <c r="B17" s="2" t="s">
         <v>124</v>
       </c>
@@ -2830,7 +2907,7 @@
       </c>
       <c r="G17" s="22"/>
     </row>
-    <row r="18" spans="2:8" ht="229.5">
+    <row r="18" spans="2:9" ht="229.5">
       <c r="B18" s="2"/>
       <c r="C18" s="12" t="s">
         <v>132</v>
@@ -2842,7 +2919,7 @@
         <v>135</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>136</v>
@@ -2851,7 +2928,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="216">
+    <row r="19" spans="2:9" ht="310.5">
       <c r="B19" s="2" t="s">
         <v>147</v>
       </c>
@@ -2862,34 +2939,35 @@
         <v>144</v>
       </c>
       <c r="E19" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="F19" s="43" t="s">
-        <v>151</v>
-      </c>
       <c r="G19" s="22"/>
-      <c r="H19" s="53" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="222" customHeight="1">
+      <c r="H19" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="I19" s="53"/>
+    </row>
+    <row r="20" spans="2:9" ht="222" customHeight="1">
       <c r="B20" s="2"/>
       <c r="C20" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="E20" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="E20" s="43" t="s">
-        <v>167</v>
-      </c>
       <c r="F20" s="43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="53"/>
     </row>
-    <row r="21" spans="2:8" ht="121.5" customHeight="1">
+    <row r="21" spans="2:9" ht="121.5" customHeight="1">
       <c r="B21" s="54"/>
       <c r="C21" s="55" t="s">
         <v>146</v>
@@ -2898,76 +2976,76 @@
         <v>145</v>
       </c>
       <c r="E21" s="56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F21" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G21" s="57"/>
     </row>
-    <row r="22" spans="2:8" ht="120.75" customHeight="1">
+    <row r="22" spans="2:9" ht="120.75" customHeight="1">
       <c r="B22" s="54"/>
       <c r="C22" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="D22" s="55" t="s">
+      <c r="E22" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="E22" s="56" t="s">
-        <v>157</v>
-      </c>
       <c r="F22" s="56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G22" s="57"/>
     </row>
-    <row r="23" spans="2:8" s="12" customFormat="1" ht="120.75" customHeight="1">
+    <row r="23" spans="2:9" s="12" customFormat="1" ht="120.75" customHeight="1">
       <c r="C23" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="E23" s="43" t="s">
-        <v>172</v>
-      </c>
       <c r="F23" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="2:9" s="62" customFormat="1" ht="81">
+      <c r="B24" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="2:8" s="63" customFormat="1" ht="81">
-      <c r="B24" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="59" t="s">
+      <c r="E24" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" s="59" t="s">
         <v>153</v>
       </c>
-      <c r="D24" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="E24" s="60" t="s">
-        <v>177</v>
-      </c>
-      <c r="F24" s="60" t="s">
-        <v>154</v>
-      </c>
-      <c r="G24" s="61"/>
-      <c r="H24" s="62"/>
-    </row>
-    <row r="25" spans="2:8" ht="94.5">
+      <c r="G24" s="60"/>
+      <c r="H24" s="61"/>
+    </row>
+    <row r="25" spans="2:9" ht="94.5">
       <c r="B25" s="2"/>
       <c r="C25" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="E25" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="E25" s="43" t="s">
-        <v>160</v>
-      </c>
       <c r="F25" s="43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G25" s="22"/>
     </row>
@@ -3105,7 +3183,7 @@
         <v>283</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="3:4">
@@ -3113,7 +3191,7 @@
         <v>285</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="3:4">
@@ -3121,7 +3199,7 @@
         <v>287</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3154,12 +3232,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="109.5" customHeight="1">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
     </row>
     <row r="3" spans="2:18">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
Add ball get_all api
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -1324,21 +1324,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>query ball base by users</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ball/get_all</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- /* the mobile that register */
- "mobile": xxxx,
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>get profile</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1474,34 +1459,6 @@
  "lat": xxx,
  "lng": xxx,
  "distance": xxx,
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
- /* the mobile that register */
- "mobile":xxx,
- "balls:":[{
-  /* the mobile that register */
-  "ball_id": xxxx,
-  /* what type of ball */
-  "type": xxx,
-  /* what content in ball */
-  "content": xxx,
-  /* the location of ball */
-  "current_lat": xxxx,
-  "current_lng": xxxx,
- },{
-  /* the mobile that register */
-  "ball_id": xxxx,
-  /* what type of ball */
-  "type": xxx,
-  /* what content in ball */
-  "content": xxx,
-  /* the location of ball */
-  "current_lat": xxxx,
-  "current_lng": xxxx,
- }]
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1658,12 +1615,130 @@
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>query ball base by users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ball/get_all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+ /* the mobile that register */
+ "mobile": xxxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /* the date that indicate the timestamp */
+ "since_date": xxxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+ /* the mobile that register */
+ "mobile":xxx,
+ "balls:":[{
+  /* the mobile that register */
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "sender": xxxx,
+  "catcher": xxxx,
+  "ball_status": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ },{
+  /* the mobile that register */
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "sender": xxxx,
+  "catcher": xxxx,
+  "ball_status": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ }]
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1837,6 +1912,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -2164,11 +2247,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2586,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2595,7 +2678,7 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="31.625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.75" style="12" customWidth="1"/>
-    <col min="5" max="5" width="40.5" style="22" customWidth="1"/>
+    <col min="5" max="5" width="44.5" style="22" customWidth="1"/>
     <col min="6" max="6" width="33.25" style="22" customWidth="1"/>
     <col min="7" max="7" width="45" customWidth="1"/>
     <col min="8" max="8" width="56.375" style="17" customWidth="1"/>
@@ -2919,7 +3002,7 @@
         <v>135</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>136</v>
@@ -2945,24 +3028,24 @@
         <v>150</v>
       </c>
       <c r="G19" s="22"/>
-      <c r="H19" s="64" t="s">
-        <v>177</v>
+      <c r="H19" s="63" t="s">
+        <v>173</v>
       </c>
       <c r="I19" s="53"/>
     </row>
     <row r="20" spans="2:9" ht="222" customHeight="1">
       <c r="B20" s="2"/>
       <c r="C20" s="12" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="53"/>
@@ -2976,41 +3059,41 @@
         <v>145</v>
       </c>
       <c r="E21" s="56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F21" s="56" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G21" s="57"/>
     </row>
     <row r="22" spans="2:9" ht="120.75" customHeight="1">
-      <c r="B22" s="54"/>
-      <c r="C22" s="55" t="s">
-        <v>154</v>
-      </c>
-      <c r="D22" s="55" t="s">
-        <v>155</v>
-      </c>
-      <c r="E22" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="F22" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="G22" s="57"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="2:9" s="12" customFormat="1" ht="120.75" customHeight="1">
       <c r="C23" s="43" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H23" s="17"/>
     </row>
@@ -3022,10 +3105,10 @@
         <v>152</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E24" s="59" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F24" s="59" t="s">
         <v>153</v>
@@ -3036,16 +3119,16 @@
     <row r="25" spans="2:9" ht="94.5">
       <c r="B25" s="2"/>
       <c r="C25" s="12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F25" s="43" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G25" s="22"/>
     </row>
@@ -3183,7 +3266,7 @@
         <v>283</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="3:4">
@@ -3191,7 +3274,7 @@
         <v>285</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="3:4">
@@ -3199,7 +3282,7 @@
         <v>287</v>
       </c>
       <c r="D17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3232,12 +3315,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="109.5" customHeight="1">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
     </row>
     <row r="3" spans="2:18">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
Add begin_date and end_date
current_loc/get_all
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -1463,42 +1463,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">{
-  /* the mobile that register */
-  "mobile":xxx,
-  "ball_id": xxxx,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  /* 0: running, 3: dead */
-  "ball_status": xxx,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-  /* the location of ball */
-  "current_lat": xxxx,
-  "current_lng": xxxx,
-}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>profile/update</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1680,7 +1644,20 @@
       </rPr>
       <t xml:space="preserve">  "sender": xxxx,
   "catcher": xxxx,
-  "ball_status": xxx,</t>
+  "ball_status": xxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "begin_date": xxx,
+  "end_date": xxx,</t>
     </r>
     <r>
       <rPr>
@@ -1714,7 +1691,20 @@
       </rPr>
       <t xml:space="preserve">  "sender": xxxx,
   "catcher": xxxx,
-  "ball_status": xxx,</t>
+  "ball_status": xxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "begin_date": xxx,
+  "end_date": xxx,</t>
     </r>
     <r>
       <rPr>
@@ -1733,12 +1723,71 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+  /* the mobile that register */
+  "mobile":xxx,
+  "ball_id": xxxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  /* 0: running, 3: dead */
+  "ball_status": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "begin_date": xxx,
+  "end_date": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1915,6 +1964,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -2669,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3029,7 +3086,7 @@
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I19" s="53"/>
     </row>
@@ -3045,7 +3102,7 @@
         <v>163</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="53"/>
@@ -3069,16 +3126,16 @@
     <row r="22" spans="2:9" ht="120.75" customHeight="1">
       <c r="B22" s="12"/>
       <c r="C22" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="E22" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="F22" s="43" t="s">
         <v>177</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>178</v>
       </c>
       <c r="G22" s="12"/>
     </row>
@@ -3093,7 +3150,7 @@
         <v>168</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H23" s="17"/>
     </row>
@@ -3105,10 +3162,10 @@
         <v>152</v>
       </c>
       <c r="D24" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" s="59" t="s">
         <v>170</v>
-      </c>
-      <c r="E24" s="59" t="s">
-        <v>171</v>
       </c>
       <c r="F24" s="59" t="s">
         <v>153</v>
@@ -3128,7 +3185,7 @@
         <v>156</v>
       </c>
       <c r="F25" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G25" s="22"/>
     </row>

</xml_diff>

<commit_message>
Add require type argument
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -1590,21 +1590,48 @@
   <si>
     <r>
       <t xml:space="preserve">{
- /* the mobile that register */
- "mobile": xxxx,
+  /* the mobile that register */
+  "mobile":xxx,
+  "ball_id": xxxx,
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> /* the date that indicate the timestamp */
- "since_date": xxxx,</t>
+      <t xml:space="preserve">  /* 0: running, 3: dead */
+  "ball_status": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="-0.499984740745262"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "begin_date": xxx,
+  "end_date": xxx,</t>
     </r>
     <r>
       <rPr>
@@ -1726,22 +1753,22 @@
   <si>
     <r>
       <t xml:space="preserve">{
-  /* the mobile that register */
-  "mobile":xxx,
-  "ball_id": xxxx,
+ /* the mobile that register */
+ "mobile": xxxx,
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="6" tint="-0.499984740745262"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  /* 0: running, 3: dead */
-  "ball_status": xxx,</t>
+      <t xml:space="preserve"> /* require type: 1, sender;2,receiver;3,
+ sender+receiver */
+ "requireType": xx;</t>
     </r>
     <r>
       <rPr>
@@ -1752,22 +1779,20 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-  /* the location of ball */
-  "current_lat": xxxx,
-  "current_lng": xxxx,
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="6" tint="-0.499984740745262"/>
+        <color rgb="FFC00000"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  "begin_date": xxx,
-  "end_date": xxx,</t>
+      <t xml:space="preserve"> /* the date that indicate the timestamp
+ of latest balls */
+ "since_date": xxxx,</t>
     </r>
     <r>
       <rPr>
@@ -2727,7 +2752,7 @@
   <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3102,7 +3127,7 @@
         <v>163</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="53"/>
@@ -3132,7 +3157,7 @@
         <v>175</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F22" s="43" t="s">
         <v>177</v>

</xml_diff>

<commit_message>
Add received balls result, and define since_date
since_date : it's timestamp that calculating since 1970
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -1745,7 +1745,59 @@
   /* the location of ball */
   "current_lat": xxxx,
   "current_lng": xxxx,
- }]
+ }],
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "received_balls:":[{
+  /* the mobile that register */
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+  "sender": xxxx,
+  "catcher": xxxx,
+  "ball_status": xxx,
+  "begin_date": xxx,
+  "end_date": xxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ },{
+  /* the mobile that register */
+  "ball_id": xxxx,
+  /* what type of ball */
+  "type": xxx,
+  /* what content in ball */
+  "content": xxx,
+  "sender": xxxx,
+  "catcher": xxxx,
+  "ball_status": xxx,
+  "begin_date": xxx,
+  "end_date": xxx,
+  /* the location of ball */
+  "current_lat": xxxx,
+  "current_lng": xxxx,
+ }]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 }</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1791,7 +1843,29 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> /* the date that indicate the timestamp
- of latest balls */
+ of latest balls, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the timestamps that from 1970 to now</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> */
  "since_date": xxxx,</t>
     </r>
     <r>
@@ -1812,7 +1886,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1997,6 +2071,14 @@
     <font>
       <sz val="11"/>
       <color theme="6" tint="-0.499984740745262"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -2752,7 +2834,7 @@
   <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
UPDATE area_scan to robot_scan
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -1576,14 +1576,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>area scan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>feed/area_scan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{
  /* the mobile that register */
  "mobile": xxxx,
@@ -1666,6 +1658,14 @@
  },
  ]
 }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>robot scan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feed/robot_scan</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2621,7 +2621,7 @@
   <dimension ref="B2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2953,7 +2953,7 @@
         <v>135</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>136</v>
@@ -2965,16 +2965,16 @@
     <row r="19" spans="2:9" ht="229.5">
       <c r="B19" s="2"/>
       <c r="C19" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="E19" s="51" t="s">
-        <v>176</v>
-      </c>
       <c r="F19" s="43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="35"/>
@@ -2993,7 +2993,7 @@
         <v>149</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="63" t="s">
@@ -3013,7 +3013,7 @@
         <v>160</v>
       </c>
       <c r="F21" s="43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="53"/>
@@ -3030,7 +3030,7 @@
         <v>161</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G22" s="57"/>
     </row>
@@ -3046,7 +3046,7 @@
         <v>170</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G23" s="12"/>
     </row>
@@ -3061,7 +3061,7 @@
         <v>164</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H24" s="17"/>
     </row>
@@ -3079,7 +3079,7 @@
         <v>166</v>
       </c>
       <c r="F25" s="59" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G25" s="60"/>
       <c r="H25" s="61"/>
@@ -3096,7 +3096,7 @@
         <v>154</v>
       </c>
       <c r="F26" s="43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G26" s="22"/>
     </row>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="E27" s="43"/>
       <c r="F27" s="43" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G27" s="22"/>
     </row>
@@ -3120,7 +3120,7 @@
       <c r="B28" s="2"/>
       <c r="E28" s="43"/>
       <c r="F28" s="43" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G28" s="22"/>
     </row>
@@ -3128,7 +3128,7 @@
       <c r="B29" s="2"/>
       <c r="E29" s="43"/>
       <c r="F29" s="43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G29" s="22"/>
     </row>
@@ -3136,7 +3136,7 @@
       <c r="B30" s="2"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G30" s="22"/>
     </row>
@@ -3144,7 +3144,7 @@
       <c r="B31" s="2"/>
       <c r="E31" s="43"/>
       <c r="F31" s="43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G31" s="22"/>
     </row>
@@ -3152,7 +3152,7 @@
       <c r="B32" s="2"/>
       <c r="E32" s="43"/>
       <c r="F32" s="43" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G32" s="22"/>
     </row>
@@ -3160,7 +3160,7 @@
       <c r="B33" s="2"/>
       <c r="E33" s="43"/>
       <c r="F33" s="43" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G33" s="22"/>
     </row>
@@ -3168,7 +3168,7 @@
       <c r="B34" s="2"/>
       <c r="E34" s="43"/>
       <c r="F34" s="43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G34" s="22"/>
     </row>
@@ -3176,7 +3176,7 @@
       <c r="B35" s="2"/>
       <c r="E35" s="43"/>
       <c r="F35" s="43" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G35" s="22"/>
     </row>

</xml_diff>

<commit_message>
ADD robot avatar url
concate avatar url with server address ip
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -1641,7 +1641,16 @@
     <t>}</t>
   </si>
   <si>
-    <t>{
+    <t>robot scan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feed/robot_scan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
  "status": 0, 
  "mobile": xxx,
  "robots": [ 
@@ -1650,22 +1659,59 @@
  /* lat and lng */
  "current_lat": xxx,
  "current_lng": xxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "avatar_url": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
  }, {
  "user": xxx
  /* lat and lng */
  "current_lat": xxx,
  "current_lng": xxx,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "avatar_url": xxx,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
  },
  ]
 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>robot scan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>feed/robot_scan</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2621,7 +2667,7 @@
   <dimension ref="B2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2962,19 +3008,19 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="229.5">
+    <row r="19" spans="2:9" ht="256.5">
       <c r="B19" s="2"/>
       <c r="C19" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>189</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>190</v>
       </c>
       <c r="E19" s="51" t="s">
         <v>174</v>
       </c>
       <c r="F19" s="43" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="35"/>

</xml_diff>

<commit_message>
ADD for continue login
</commit_message>
<xml_diff>
--- a/docs/API_Intro_V4.xlsx
+++ b/docs/API_Intro_V4.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="192">
   <si>
     <t>check if register</t>
   </si>
@@ -1710,6 +1710,37 @@
       <t xml:space="preserve">
  },
  ]
+}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+ "status": 0,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> //continue login count: 0 for nothing, &gt; 0 for continue login
+ "count": x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 }</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2666,8 +2697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2758,7 +2789,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>17</v>

</xml_diff>